<commit_message>
VISTA-5923: Preload at least four buildings for the same city in case of DEMO to show properly on site app - Added more US addresses - Added and updated more Canada addresses - Added more building marketing descritpions
</commit_message>
<xml_diff>
--- a/vista-dev/vista-dev-generator/src/main/resources/com/propertyvista/generator/util/buildings.xlsx
+++ b/vista-dev/vista-dev-generator/src/main/resources/com/propertyvista/generator/util/buildings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="72" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="52" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
   <si>
     <t>name</t>
   </si>
@@ -37,37 +37,37 @@
     </r>
   </si>
   <si>
-    <t>Parkways on Prairie Creek Apartments are located on Memorial Avenue inside Houston's 610 Loop only minutes from downtown and steps away from Memorial Park. The main throughway is Memorial Avenue so even during peak rush hour your trip to Downtown Houston is quick and unhindered. Loops 610, I-10 and I-45 are quickly accessible from our great location. This location just cant be beat! </t>
+    <t>Parkways on Prairie Creek Apartments are located on Memorial Avenue inside Houston's 610 Loop only minutes from downtown and steps away from Memorial Park. The main throughway is Memorial Avenue so even during peak rush hour your trip to Downtown Houston is quick and unhindered. Loops 610, I-10 and I-45 are quickly accessible from our great location. This location just cant be beat!</t>
   </si>
   <si>
     <t>Golden Mile</t>
   </si>
   <si>
-    <t>Discover luxurious apartment living that offers you everything you are looking for: beauty, comfort and convenience. If you are looking for sophistication, warmth, and a sense of community, you have come to the right place. </t>
+    <t>Discover luxurious apartment living that offers you everything you are looking for: beauty, comfort and convenience. If you are looking for sophistication, warmth, and a sense of community, you have come to the right place.</t>
   </si>
   <si>
     <t>Gallery at Turtle Creek</t>
   </si>
   <si>
-    <t>The Ascent at CITYCENTRE Luxury Apartments are brand new, exciting residences designed by prominent architects and interior designers in the Houston area. Learn more about apartments available for rent in West Houston. </t>
+    <t>The Ascent at CITYCENTRE Luxury Apartments are brand new, exciting residences designed by prominent architects and interior designers in the Houston area. Learn more about apartments available for rent in West Houston.</t>
   </si>
   <si>
     <t>The Metropolitan</t>
   </si>
   <si>
-    <t>Meet Astor and get to know Houston living the way it's supposed to be. You know exactly what we mean. First, it's about the location. The perfect, unbelieveable location in the toney Tanglewood neighborhood - hands-down one of Houston's preeminent neighborhoods, and home to the Houston Country Club as well as many prominent Houstonians (like President George H.W. Bush - you may just run into him or Babs at the grocery!). </t>
+    <t>Meet Astor and get to know Houston living the way it's supposed to be. You know exactly what we mean. First, it's about the location. The perfect, unbelieveable location in the toney Tanglewood neighborhood - hands-down one of Houston's preeminent neighborhoods, and home to the Houston Country Club as well as many prominent Houstonians (like President George H.W. Bush - you may just run into him or Babs at the grocery!).</t>
   </si>
   <si>
     <t>The Arches at Park Cities</t>
   </si>
   <si>
-    <t>It’s more than just a residence, 1000 Jefferson is an impressive luxury apartment community offering exceptional services and sophisticated interior design. 1000 Jefferson’s contemporary main lobbies, designed in fine Italian marble, marks where the heart of Hoboken becomes your home. 1000 Jefferson offers spacious one, two and three bedroom apartment homes. In addition to our spa featured pool furnished with lounge chairs, our community offers a Rooftop with dramatic Manhattan skyline views, 24 hour Fitness Club with State-of-the-Art equipment, WiFi-enabled Resident Lounge and private garage parking. </t>
+    <t>It’s more than just a residence, 1000 Jefferson is an impressive luxury apartment community offering exceptional services and sophisticated interior design. 1000 Jefferson’s contemporary main lobbies, designed in fine Italian marble, marks where the heart of Hoboken becomes your home. 1000 Jefferson offers spacious one, two and three bedroom apartment homes. In addition to our spa featured pool furnished with lounge chairs, our community offers a Rooftop with dramatic Manhattan skyline views, 24 hour Fitness Club with State-of-the-Art equipment, WiFi-enabled Resident Lounge and private garage parking.</t>
   </si>
   <si>
     <t>The Gate in The Village</t>
   </si>
   <si>
-    <t>TRIO Apartments brings you a taste of New Urbanism. These luxury apartments in Pasadena, CA are designed with respect for the city’s past, present and future, with an elegantly appointed five-story Colorado Boulevard community will bring you into a world of its own. TRIO Apartments have converted Pasadena’s first parking garage into a charming, historical Recreation/Leasing Center, and preserved other nearby buildings of historical significance. Stop by today and allow TRIO to sweep you away! </t>
+    <t>TRIO Apartments brings you a taste of New Urbanism. These luxury apartments in Pasadena, CA are designed with respect for the city’s past, present and future, with an elegantly appointed five-story Colorado Boulevard community will bring you into a world of its own. TRIO Apartments have converted Pasadena’s first parking garage into a charming, historical Recreation/Leasing Center, and preserved other nearby buildings of historical significance. Stop by today and allow TRIO to sweep you away!</t>
   </si>
   <si>
     <r>
@@ -84,7 +84,7 @@
     </r>
   </si>
   <si>
-    <t>Holly Street Village is situated in the heart of charming, picturesque Old Town Pasadena a splendid, historic neighborhood, where people take joy in strolling, dining and mingling in a mellow, outdoor, urban setting full of wonders. Located within walking distance of Paseo Colorado, residents of Holly Street Village enjoy an exquisite collection of sidewalk cafes, galleries, theaters and some of the finest dining and shopping in the Greater Los Angeles Area. Home to the extravagance of the world-famous Tournament of Roses Parade and the Rose Bowl game, you will find entertainment, culture and art at every turn. </t>
+    <t>Holly Street Village is situated in the heart of charming, picturesque Old Town Pasadena a splendid, historic neighborhood, where people take joy in strolling, dining and mingling in a mellow, outdoor, urban setting full of wonders. Located within walking distance of Paseo Colorado, residents of Holly Street Village enjoy an exquisite collection of sidewalk cafes, galleries, theaters and some of the finest dining and shopping in the Greater Los Angeles Area. Home to the extravagance of the world-famous Tournament of Roses Parade and the Rose Bowl game, you will find entertainment, culture and art at every turn.</t>
   </si>
   <si>
     <r>
@@ -103,7 +103,7 @@
     </r>
   </si>
   <si>
-    <t>The Renaissance Terrace Apartments For Rent in Long Beach, California is centrally located in the heart of downtown Long Beach and within walking distance of Pine Avenue and the East Village District. Shop at City Place, dine at Shoreline Village, or take a relaxing stroll along the waterfront. Come experience carefree contemporary living in our newly renovated one-, two- and three-bedroom apartment homes. Our Renaissance Terrace pet friendly apartments in Long Beach, California welcomes your four-legged friend. </t>
+    <t>The Renaissance Terrace Apartments For Rent in Long Beach, California is centrally located in the heart of downtown Long Beach and within walking distance of Pine Avenue and the East Village District. Shop at City Place, dine at Shoreline Village, or take a relaxing stroll along the waterfront. Come experience carefree contemporary living in our newly renovated one-, two- and three-bedroom apartment homes. Our Renaissance Terrace pet friendly apartments in Long Beach, California welcomes your four-legged friend.</t>
   </si>
   <si>
     <r>
@@ -120,7 +120,7 @@
     </r>
   </si>
   <si>
-    <t>Get the lifestyle you deserve at Riverbend. You`ll love your spacious one or two bedroom apartment homes. At Riverbend, you`ll enjoy an array of amenities including multi-level swimming pool, year round Jacuzzi, gym, and business center with free internet. With our convenient location close to freeway entrances, TRAX, dining, shopping and entertainment, you`re sure to be impressed! Visit Riverbend today! </t>
+    <t>Get the lifestyle you deserve at Riverbend. You`ll love your spacious one or two bedroom apartment homes. At Riverbend, you`ll enjoy an array of amenities including multi-level swimming pool, year round Jacuzzi, gym, and business center with free internet. With our convenient location close to freeway entrances, TRAX, dining, shopping and entertainment, you`re sure to be impressed! Visit Riverbend today!</t>
   </si>
   <si>
     <r>
@@ -137,25 +137,25 @@
     </r>
   </si>
   <si>
-    <t>Our urban apartment homes in Long Beach put a fresh spin on rental living, with 129 modern units that include one- and two- bedroom and studio floor plans styled by noted designers for aesthetic-minded people like you. We feature prime amenities such as our amazing downtown location with open layouts, nine-foot ceilings, large closets and a fitness center. All of these and our many other offerings give you the services you need to live a life of luxury; apply online now. </t>
+    <t>Our urban apartment homes in Long Beach put a fresh spin on rental living, with 129 modern units that include one- and two- bedroom and studio floor plans styled by noted designers for aesthetic-minded people like you. We feature prime amenities such as our amazing downtown location with open layouts, nine-foot ceilings, large closets and a fitness center. All of these and our many other offerings give you the services you need to live a life of luxury; apply online now.</t>
   </si>
   <si>
     <t>The Ridge</t>
   </si>
   <si>
-    <t>Marina del Rey Apartments in Los Angeles is located between Venice Beach and Playa Vista. We are steps to the beach and surrounded by unique shopping and dining. Our newly renovated homes feature white kitchen and bath cabinetry, new granite counters, stainless steel Whirlpool appliances, engineered wood flooring and an upgraded lighting package. Our floor plans offer spacious closets, in-home washer/dryer and private patio/balcony with ocean, marina and city views. Enjoy our fitness center, resort-style pool and spa, tennis courts and dog park. Nearby recreational activities include para-sailing, sport fishing, harbor cruises, jet skiing, kayaking, paddle boarding and bike trails </t>
+    <t>Marina del Rey Apartments in Los Angeles is located between Venice Beach and Playa Vista. We are steps to the beach and surrounded by unique shopping and dining. Our newly renovated homes feature white kitchen and bath cabinetry, new granite counters, stainless steel Whirlpool appliances, engineered wood flooring and an upgraded lighting package. Our floor plans offer spacious closets, in-home washer/dryer and private patio/balcony with ocean, marina and city views. Enjoy our fitness center, resort-style pool and spa, tennis courts and dog park. Nearby recreational activities include para-sailing, sport fishing, harbor cruises, jet skiing, kayaking, paddle boarding and bike trails</t>
   </si>
   <si>
     <t>The Palms</t>
   </si>
   <si>
-    <t>The Brooklyner known as the tallest building in the borough, is located at 111 Lawrence Street and offers apartments in downtown Brooklyn. Choose from efficient and modern Brooklyn apartments designed with Italian cabinetry, granite countertops, stainless steel appliances, hardwood floors, solar window shades, and stellar views. Residents can take advantage of the beautiful rooftop sundeck and lounge, the resident Lodge, on-site valet parking, bike storage and more! The new residential neighborhood lies at the core of Brooklyn Heights, DUMBO, Fort Greene, Boerum Hill, Cobble Hill and Carroll Gardens. Restaurants and shops are emerging on every corner and just about every subway line is accessible within 3 blocks. </t>
+    <t>The Brooklyner known as the tallest building in the borough, is located at 111 Lawrence Street and offers apartments in downtown Brooklyn. Choose from efficient and modern Brooklyn apartments designed with Italian cabinetry, granite countertops, stainless steel appliances, hardwood floors, solar window shades, and stellar views. Residents can take advantage of the beautiful rooftop sundeck and lounge, the resident Lodge, on-site valet parking, bike storage and more! The new residential neighborhood lies at the core of Brooklyn Heights, DUMBO, Fort Greene, Boerum Hill, Cobble Hill and Carroll Gardens. Restaurants and shops are emerging on every corner and just about every subway line is accessible within 3 blocks.</t>
   </si>
   <si>
     <t>Reserve at Arrowhead</t>
   </si>
   <si>
-    <t>Teresina apartments are located minutes from the Pacific Ocean, offering elegant hilltop living overlooking beautiful Otay Ranch. Teresina apartments welcome large dogs and are within walking distance to schools. Easy freeway access from Teresina apartments ensures that you'll be at your favorite restaurants and shops in no time. Come check out everything Teresina apartments have to offer! </t>
+    <t>Teresina apartments are located minutes from the Pacific Ocean, offering elegant hilltop living overlooking beautiful Otay Ranch. Teresina apartments welcome large dogs and are within walking distance to schools. Easy freeway access from Teresina apartments ensures that you'll be at your favorite restaurants and shops in no time. Come check out everything Teresina apartments have to offer!</t>
   </si>
   <si>
     <r>
@@ -174,7 +174,7 @@
     </r>
   </si>
   <si>
-    <t>iberty Park Apartments in Braintree, MA is a newly renovated community located close to Boston and 30 minutes from Cape Cod. We provide easy access to Routes 93, 95 and 3, while still maintaining a park-like setting. Liberty Park is convenient to great shopping and dining and we also provide a private shuttle to the Braintree T Station. Our apartments feature in-home washers and dryers, spacious closets and fireplaces. Residents will also enjoy working out in the fitness center and relaxing at the pool. You can also take advantage of the nearby local parks, walking trails and the Stoddard dog park as well as being part of excellent Braintree School District. </t>
+    <t>iberty Park Apartments in Braintree, MA is a newly renovated community located close to Boston and 30 minutes from Cape Cod. We provide easy access to Routes 93, 95 and 3, while still maintaining a park-like setting. Liberty Park is convenient to great shopping and dining and we also provide a private shuttle to the Braintree T Station. Our apartments feature in-home washers and dryers, spacious closets and fireplaces. Residents will also enjoy working out in the fitness center and relaxing at the pool. You can also take advantage of the nearby local parks, walking trails and the Stoddard dog park as well as being part of excellent Braintree School District.</t>
   </si>
   <si>
     <r>
@@ -193,7 +193,433 @@
     </r>
   </si>
   <si>
-    <t>Your newly renovated apartment home at Promenade at Aventura, includes GE appliances, upgraded countertops and brand new kitchen cabinets. Our beautiful community overlooks the fairways of the Turnberry Country Club in Aventura, FL. We are located adjacent to great dining and shopping at the Aventura Mall, and are minutes from the Intracostal Waterway and the Atlantic coast. </t>
+    <t>Your newly renovated apartment home at Promenade at Aventura, includes GE appliances, upgraded countertops and brand new kitchen cabinets. Our beautiful community overlooks the fairways of the Turnberry Country Club in Aventura, FL. We are located adjacent to great dining and shopping at the Aventura Mall, and are minutes from the Intracostal Waterway and the Atlantic coast.</t>
+  </si>
+  <si>
+    <t>The Dovercourt</t>
+  </si>
+  <si>
+    <t>A Loft-Inspired Condo Residence, Where Thoughtful Design And Utilization Of Space Allow For Great Comfort And Luxurious Living. This Is A Premium Corner Unit With Both Bedrooms Having Windows. Includes One Parking And One Locker Taxes Has Not Been Assessed Yet. </t>
+  </si>
+  <si>
+    <t>The Townhouse</t>
+  </si>
+  <si>
+    <t>Bright And Spacious Corner Unit, Approximately 1326 Sq. Ft. Features Include Rooftop Terrace, Juliette Balcony Off The Master Bedroom, Walk-In Closet And 3 Pc Ensuite. Freshly Painted, New Laminate Throughout, Newly Sanded Parquet Floor, Underground Owned Parking And Locker, Easy Access To Visitor Parking. Convenient Location Close To Go And Subway. </t>
+  </si>
+  <si>
+    <t>Matheson Corner</t>
+  </si>
+  <si>
+    <t>Brand New Building Never Lived In. Fantastic Corner Unit With Amazing South East Views. Great Layout With Double Closet In Foyer, Wide Plank Laminate In L/R And D/R. Kitchen Boasts Beautiful Floor Tile That Compliments The Granite Counters, Dark Cabinets And Stainless Steel Appliances Including Over The Range Micro/Hood Combo. Don't Miss This Opportunity To Live In A Great Bldg Close To Amenities And Shopping. Near High Park And Close To Shopping. </t>
+  </si>
+  <si>
+    <t>Sunset Condominium</t>
+  </si>
+  <si>
+    <t>Beautiful Heritage Building. 2 Storey Lofts are Sure To Impress W/ Soaring 16.5' Ceilings, 5" Wide Plank Pine Floors, Exposed Ductwork &amp; Original Industrial Beams. Unbelievable Master On Mezzanine With W/I Closet And 4 Pc Ensuite. Open Concept Kitchen &amp; Dining W/ Ss Appliances And A Modern White Kitchen. Under Stairs Could Make A Great Office! </t>
+  </si>
+  <si>
+    <t>The Iron Works Lofts</t>
+  </si>
+  <si>
+    <t>Boutique Loft Building With Only 15 Units.Soaring 11Ft High Ceilings!Real Hardwood Floors &amp; Designer Kitchen With Granite Counter Tops &amp; Back-Splash,B/Fast Bar &amp; Stainless Appliances.Fabulous Bright Open Space.Dining Room Features A Large Feature Stone Wall With A Fireplace.2 Large Private Bedrooms.Building Features A Charming 350 Sqft Shared Terrace.Short Walk To  Subway &amp; Mall.One Parking Space Included </t>
+  </si>
+  <si>
+    <t>Red Hot Building</t>
+  </si>
+  <si>
+    <t>Rare Corner South West Exposure, Elegant 2 Br, 2 Bath ( 857 Sq F + 49 Sq F Balcony) Units In 12 Storey Boutigue Midrise Across From the City's Biggest Urban Park! The Building Has A Dog Spa, Fitness, Terrace Venue. Minutes Away From The Subway, Shops And Restourants, Banks, Pharmacies, Animal Hospital, Dental Office. The Best Schools, Easy Access To The Highway And Much More </t>
+  </si>
+  <si>
+    <t>Sandy's Apartments</t>
+  </si>
+  <si>
+    <t>Stunning 2 Bedroom, 2 Bath Condos Overlooking biggest Park in the city. Ideally Located Close To Trendy Markets And The Entertaining neighborhood. Steps From Public Transport And Major Transportation Routes. Bedrooms Are Located On Either Side Of The Unit And Have Separate Bathrooms; Ideal For Investors. </t>
+  </si>
+  <si>
+    <t>Sensations</t>
+  </si>
+  <si>
+    <t>Vibrant, Amazing &amp; Popular Split Two Bedroom With Fantastic View Of The City. Modern &amp; Fresh 670 Sqf Of Living Space With Efficient Design Layout. High Floor &amp; With One Parking &amp; Locker. Steps To Main Subway stops, Village And Boutique Shops, Restaurants, Schools And 24 Hrs Ttc. Walk/Transit.</t>
+  </si>
+  <si>
+    <t>Lynn Property</t>
+  </si>
+  <si>
+    <t>Spacious 771 Sq. Foot Condos. 2 Bedroom, 2 Bath, Open Concept, Kitchen Overlooks Liv Rm/Din Rm. Walkout To Balcony From Liv Rm. Master Bedroom Features Large Closet, Ensuite 4 Pc Bathroom &amp; Balcony Off Master Bedroom. Stainless Steel Appliances Plus Washer/Dryer. Many Amenities Including Indoor Pool, Underground Parking, Billiards Room, Media/Theatre Room, Exercise Room, Guest Suites. A Great Opportunity.</t>
+  </si>
+  <si>
+    <t>Jeffrey Condominium</t>
+  </si>
+  <si>
+    <t>A Gem In Village. Amazing Sub-Penthouse Customized Condo Units Unique To Entire City. Just Under 1000 Sqft Of Interior Space With An 828 Sqft Private Terrace! Entertain 100 Friends &amp; Family! Enjoy A Combined Living/Cooking/Dining Area Including A Beautiful Kitchen With Matching Island. 9Ft Ceilings Throughout. 2 Bedrooms (Each With Walk-In Closets) &amp; 2 Bathrooms. Views Also To The City! Easy Parking On P1! </t>
+  </si>
+  <si>
+    <t>The City Patterns</t>
+  </si>
+  <si>
+    <t>Luxury Living In Modern Village. Bring Your Pickiest Clients, This Layout Is Fantastic! Gorgeous Open Concept, Two Bedroom Suites. Steps From Trendy Restaurants And Shops. Extremely Convenient Location With Access To Transit &amp; Highways. Bring Your Entire Wardrobe, Master Has A Huge Walk In Closet! Great Opportunity With Fantastic Revenue For An Investor Or Move In Yourself. Currently Rented To A + Tenants Who Are Willing To Stay. Parking &amp; Locker Also Rented </t>
+  </si>
+  <si>
+    <t>The Rainbow</t>
+  </si>
+  <si>
+    <t>Stunning 2Bdrm Corner Units In Fabulous Liberty Village W/Two Huge Balconies &amp; An Amazing Unobstructed Downtown Skyline View. Fantastic Floorplan W/Two Full Baths! Upgraded To Suit The Pickiest Buyer! Hardwood Flrs Throughout, Floor To Ceiling Wrap Around Windows, Open Modern Kitchen W/Glass Backsplash, Granite Countertops &amp; A Center Island With Breakfast Bar, Stainless Steel Appliances, &amp; Two Huge Balconies With Million Dollar City Views! Unit Comes W/Parking </t>
+  </si>
+  <si>
+    <t>Stafford Apartments</t>
+  </si>
+  <si>
+    <t>Highly Coveted &amp; Rarely Available 2 Bedroom Corner Suites In The Popular Wellington Sq. Suites Offer Large Master Bedroom, Spectacular Views Through Floor To Ceiling Windows In The Living/Dining Room &amp; Master Bedroom. Beautiful Modern Open Concept Kitchen With Window. Fabulous Wrap Around Balcony With 2 Entrances. Freshly Painted. Low Maintenance Fees. Heated Locker. Great Neighbourhood. Steps Shopping &amp; Hwys. </t>
+  </si>
+  <si>
+    <t>Stanley Road Condominium</t>
+  </si>
+  <si>
+    <t>Never Before Offered "Stanley" Model 955 Sqft Of Interior Space, Highlighted By 60' Of Windows. Marble And Porcelain Bath And Ensuite, Granite Counter Open Concept Kitchen And Breakfast Bar, With Upg Custom Closets And Hunter Douglas's Top Grade Roller Shades. Very Well Maintained Building With A Long List Of Amenities. 2 Parking Spaces Makes This Unit Something Special. Free Wifi In The Lobby! </t>
+  </si>
+  <si>
+    <t>Nicole &amp; John Lofts</t>
+  </si>
+  <si>
+    <t>Westside Lofts!! Amazing Locations! 1, 2 and 3 Bedrooms, 11' Ceilings Thru Out, Hardwood Floors, Great Layout With Industrial Loft Finishes. Locker On The Same Floor As The Units Add To The Convenience! Great Roof Top Patio W/Bbq's,Well Managed Building With 24 Hr Concierge! Steps To To Everything! Public Transport At Your Door, Entertainment, Restaurants, Cafes, Shopping, Parks And More! </t>
+  </si>
+  <si>
+    <t>The Real Condo</t>
+  </si>
+  <si>
+    <t>Premier Units. Beautiful Upgraded Condo With Two or Three Bedrooms, Two Baths &amp; Stunning Views. Wall To Wall Windows. Designer Furnishes Throughout. Marble Floors In The Living &amp; Dining Room. Custom Granite Counter &amp; Backsplash, Custom Roller Blinds Throughout. Newly Painted. Large Balcony &amp; Breathtaking City/Cn Tower &amp; Lake Views From Every Room. Over 800 Square Feet Of Living Space With No Wasted Space! </t>
+  </si>
+  <si>
+    <t>Luxury on the City</t>
+  </si>
+  <si>
+    <t>This is a Pre-Construction and Pre- launch VIP Agent offer to purchase in Downtown's most exciting new development condos. Our Pick : 2 Bedroom + 2 Full Bath – Great Layout Suite. Great for Living and Investors. Reputed builder This project has been on the TEAM Paliwal radar since January. This is our project of the FALL of 2014 and we believe VERY strongly that this project is a winner. </t>
+  </si>
+  <si>
+    <t>Glamour State Building</t>
+  </si>
+  <si>
+    <t>Luxury From An Upscale Project-Water Park City Situated In A Most Desirable Area Within Short Walking Distance To City's Harbourfront, Bus, Car To Union Station, Exhibition Place, Marina, World Class Restaurants. Enjoy A Modern Kit W/S/S Appl., Lrg Liv/Din Area W/Glamourous Hrdwd Floros *Roof Top Garden,Deck With Bbq. Two, Three and Four Bedroom +Den With 2 Full Washrooms, </t>
+  </si>
+  <si>
+    <t>Luxury Neptune</t>
+  </si>
+  <si>
+    <t>Spectacular Breath-Taking Lake/Water View! Luxury Neptune At Waterpark City. Sunny Units With Beautiful Finishes, Park, Ttc Steps Away. 1, 2 and 3 Br Units With South-South/West View To Lake &amp; Park. Bright &amp; Spacious Windows &amp; Balcony. Granite Counter Top. 1 Locker &amp; 1 Parking Just Next To Entrance, Unbelievably Clear View, Show With Confidence!, Motivated Seller, Please Bring Any Offer!!! </t>
+  </si>
+  <si>
+    <t>The Crossroad</t>
+  </si>
+  <si>
+    <t>Spectacular 25th Floor Building! Suites With 2 Bedrooms + 2 Washrooms, 741 Sq Ft ! Gourmet Granite Kitchen W/Stainless Appliances Overlooking Large Living/Dining Area. Floor To Ceiling Windows, Slick Engineered Floors, Impeccably Chic Urban Design For Your High-End City Lifestyle. Top Shelf Amenities Including Health Centre, Billiards, Guest Suites, Party Room, Billiards. A Gem In The Heart Of The City !!! </t>
+  </si>
+  <si>
+    <t>The Cityplace</t>
+  </si>
+  <si>
+    <t>Brand New Luxury Cityplace with 1, 2 or 3 Bedrooms,Sw Lake View Condo Units, 24 Hrs Concierge,High Speed Internet,Steps To Ttc,Banks,Supermarket &amp; All Other Urban Convenience.Face To Canoe Landing Park,Sobeys, Minutes To Higways. Super Recreational Facilities, Indoor Gym Basketball &amp; Upscale Party Room. </t>
+  </si>
+  <si>
+    <t>The Panoramic</t>
+  </si>
+  <si>
+    <t>Panoramic City View. 1 or 2 Bdrm Condos In Financial/Entertainment/Fashion District. Luxury Quality Living, Eco Friendly Materials. 9' Ceiling, Hardwood Floor, 2 Full Washrooms, 1 Parking, 1 Locker. $$$ Upgrade. Stainless Steel Appl. Floor To Ceiling, Wall To Wall Windows. Well Maintained Shows 10+++. </t>
+  </si>
+  <si>
+    <t>The Joe's Corner</t>
+  </si>
+  <si>
+    <t>Superb Condo Community With Unrivaled Amenities And Recreation (Free Yoga &amp; Fitness Classes!) Fully Up-Graded 2,3 or 4 Bedroom, 2 Bathroom Suite With High End Finishes And Very Desirable Layout. Hardwood Floors, Southern Exposure With Park And Lake View. Walk Score 93! Steps To Starbucks And Grocery Store. Across From Canoe Landing Park. Private Balcony. Locker And Parking Spot Incl. Excellent Opp. For Ownership Or Investment. Click Tour For More Pics. </t>
+  </si>
+  <si>
+    <t>The Parade</t>
+  </si>
+  <si>
+    <t>Over 1200Sqf Luxurious Parade Condo. Bright 1 to 3 Br+Den Corner Units. Appealing Layout.Upgraded Kitchen &amp; Bath.9' Ceiling.Unobstructed Lake &amp; Park View.Close To All Amenities,Banks,Transit,Shops,Restaurants. </t>
+  </si>
+  <si>
+    <t>Forest Hill</t>
+  </si>
+  <si>
+    <t>Fantastic Opportunity To Live In This Forest Hill Luxuriously Spacious 1400 Sq. Ft. Plus Suite, Boasting 3 Bdrms, 2 Full Bthrms, 100 Sq. Ft. Balcony, Prking/Locker. Lrg Mster, With Ensuite, Dble Closet &amp; Sitting Area. Open Concept Lvng/Dining Entertainer's Delight. Amenities In This Pet-Friendly Bldg, 24Hr Concierge, Indoor Pool, Exercise Room, Game Room, Meeting Room, Sauna, Rooftop Garden And Sun Deck &amp; Guest Prking. Steps Dining/Shopping/Schools/Transit. </t>
+  </si>
+  <si>
+    <t>The Prime</t>
+  </si>
+  <si>
+    <t>Save Elevator Waiting In The Rush,Wlk To 3 Subways. Gov.Bldgs,Hospitals,University, Ryerson, Manulife Shpng Cntre Just Beside.Ttc at Your Door,Most Convenient Downtown Living. It's Best! Fantastic Views.2 Bds +2 Bths +Prkg, Lckr +Balcony,Well Kept Building.Condo. Heat/Hydro.</t>
+  </si>
+  <si>
+    <t>The Burano</t>
+  </si>
+  <si>
+    <t>Model Spacious 1196 Sq.Ft. 2 Bdrm Plus Den Corner Suites At The Burano With Spectacular N/E Views Of The Lake &amp; City Accentuated By Floor To Ceiling Windows &amp; An Open Concept Design. Over 10K Spent In Upgrades. Ideally Located In The Downtown Core Near Shops, Restaurants &amp; The University. Excellent Building Amenities Incl. An Outdoor Pool, Roof Deck &amp; 24 Hr Concierge</t>
+  </si>
+  <si>
+    <t>The Sharabi</t>
+  </si>
+  <si>
+    <t>Luxurious Suites with 2 Balconies Upgraded W/ High End Built-In Appliances, Corian Counter Top, Island, Etc.9' Smooth Ceilings. Engineered Hardwood. Parking And Locker. Multi Million Dollar Amenities. Steps To Subway,  Hospitals. High Demand Location In The Core Of Downtown. </t>
+  </si>
+  <si>
+    <t>The Sunny Hill</t>
+  </si>
+  <si>
+    <t>Large Open Bright Spacious Cityplace Condos with 2 Bedroom 2 Bathroom + Study Condo Suite. About 930 Square Feet Of Living Space + Walk-Out Balcony. Gorgeous Floors, Ensuite Laundry, 1 Tandem Parking Space That Can Fit 2 Cars + 1 Storage Locker. Full Access To All Amenities Including Pool &amp; Exercise Room. 24 Hour Concierge &amp; Visitor Parking. Close To Highways, Grocery, Shopping, Medical. </t>
+  </si>
+  <si>
+    <t>The Lakeshore</t>
+  </si>
+  <si>
+    <t>2 Bedroom Corner Units By The Lake! Enjoy Breathtaking Panoramic Views Of The Lake, High Park+City Skyline! 9 Ft Ceiling, Open Concept Gourmet Kit,Kit W/ Granite Tops, Glass Backsplash, Ss Appls.Full Length Balcony, Flr To Ceiling Windows. </t>
+  </si>
+  <si>
+    <t>The Moon Light</t>
+  </si>
+  <si>
+    <t>1, 2 and 3 Bed, 2 Bath Suites! 9' Ceilings, Floor To Ceiling Windows, Balcony. Great Views Of Lake. Great Building Amenities: 2 Pools, Tennis Court, 2 Gyms, Movie Theatre, Party Rm, Guest Suites &amp; 24Hr Security &amp; Concierge. Great Value! Steps To Lake, High Park. </t>
+  </si>
+  <si>
+    <t>The Old City Place</t>
+  </si>
+  <si>
+    <t>These Bright &amp; Spacious 2 Bedroom 1450 Sqft Units Are Steps From Old City place. This Wonderful Location Offers Subways, Parks, Schools, Shopping &amp; Dining. Only 4 Units Per Floor. There Is 24Hr Concierge Service &amp; Visitor Parking. </t>
+  </si>
+  <si>
+    <t>City Garden Place</t>
+  </si>
+  <si>
+    <t>Great Location! Formerly The Waldorf Astoria, Converted Into Luxury Condos. 2 Bdr, 2 Bath, 2 Level Penthouses. Clean, Bright, Wood Flooring Throughout, Freshly Painted, Wooden Staircase, New Stainless Steel Appliances, Skylight, Walk To Shopping, Restaurants, Cafes Within City's Trendy Neighbourhood </t>
+  </si>
+  <si>
+    <t>The Sky</t>
+  </si>
+  <si>
+    <t>2 bedrooms w/ 2 baths units. Unobstructed and panoramic view from Downtown through These unit features: new flooring, new paint, extended living room, gas stove,granite countertops. Panoramic view, enjoy the beautiful sunset &amp; easy BBQ'ing from your balcony off from the kitchen! Convenient location; steps to seabus, public transit, shopping &amp; Public Market, good dining, sea walk &amp; beautiful waterfront park. Maintenance fee includes hot water and HEAT! </t>
+  </si>
+  <si>
+    <t>The Princess</t>
+  </si>
+  <si>
+    <t>Opportunity to own a premium unit at The Sky. Perched high above the surrounding buildings and nicely renovated with hardwood floors, plush carpet, designer wall colors, 9' ceilings, new stainless steel gas range, a huge master bedroom, large balcony, and updated en-suite. Superb restaurants, shopping, , Waterfront Park, and the bus at your doorstep. Come home to World Class views of snow capped mountains, city lights, and City Bridge. Pets and rentals welcome. </t>
+  </si>
+  <si>
+    <t>The Garden Village</t>
+  </si>
+  <si>
+    <t>Immaculate two bedroom units in the prestigious Garden Village Tower. This upgraded units feature stunning hardwood floors, granite countertops, gas cooktop, s/s appliances and fireplace. Situated in the heart of High Park and just steps to highway and bus. Westely views over mountains and lake shore. Good sized covered balcony easily accomodates your BBQs. One storage locker and parking space. </t>
+  </si>
+  <si>
+    <t>The Sky Tower</t>
+  </si>
+  <si>
+    <t>Sky Tower in the heart of downtown. Prime location near bus, shops &amp; restaurants &amp; only steps to the "New Development". Beautiful units with a big balcony facing Mountains. Very functional floor plan with surprisingly big bathroom and plenty of storage space. Floor to ceiling windows. Move in today to enjoy Downtown most desirable waterfront dynamic and vibrant life style! One parking &amp; one locker. Very convenient and quiet with a walking score of 93 out of 100. It is a Walker's Paradise so daily errands do not require a car. Nearby parks. A must see! Call for showings. </t>
+  </si>
+  <si>
+    <t>The Harbour Condominium</t>
+  </si>
+  <si>
+    <t>Fabulous harbour, garden and city views from this South facing condominium. Welcome to popular tower in Lower Harbour. Open floor plan, granite countertop, engineered floor, stainless steel appliances. Soaker tub &amp; stand-up shower, fireplace with a spacious balcony of approx 86 sqft, that allows BBQ. In-suite laundry, storage and parking. Full gym facilities. Just few steps away from main streets,bus, shopping, restaurants, theatre, transit, recreation centre. Showings with a 24 hr notice. </t>
+  </si>
+  <si>
+    <t>The Pine Forest</t>
+  </si>
+  <si>
+    <t>Luxurious residences! The suites design is timeless. It features a bright open floor plan w/2 beds &amp; 2 baths. Upscale renovations include engineered hardwood floors, updated kitchen and bathrooms and plenty of built-in storage. Meticulously maintained, there is nothing to do but move in. There is a good sized balcony with views of the NS mountains and city lights. The building facilities include a full gym, 2 saunas, residential library, social room, work shop and bike room. Located in trendy area. Walking distance to various shops; groceries, coffee, ice cream, theatre, rec centre and plenty of restaurants to choose from, bus and public transportation. This location cannot be beat! </t>
+  </si>
+  <si>
+    <t>The Yellow Town</t>
+  </si>
+  <si>
+    <t>This is the PERFECT units to run a small business out of. Offering soaring 13 foot ceilings, a great open plan that's ideal for the casual entertainer, features include, easy care slate tile thru out, granite counter tops, stainless steel appliances, and to top it all off, a huge 300 sqft patio, perfect for summer barbecuing. Parking is right out your back door, and pets are allowed without restrictions. Don't miss this rare opportunity to become part of the fastest growing community. </t>
+  </si>
+  <si>
+    <t>The Terrace</t>
+  </si>
+  <si>
+    <t>Units truly like nothing else ever before available on the North Shore. Private Rooftop Patio with over 3700 sqft of combined indoor/outdoor living space. Incredible Southwestern views and exposure that is sure to please and impress the most discerning of buyers. A turn key lifestyle, with side by side parking spots with 5 star amenities available at your front door. Floor plans &amp; details package available. </t>
+  </si>
+  <si>
+    <t>The Coronado</t>
+  </si>
+  <si>
+    <t>Spacious 1, 2 and 3 bedroom and den at the Coronado, conveniently located in downtown! Beautiful earthy slate floors mixed with golden hardwood make this open and spacious layout come to life. Chat with guests while preparing a feast in this airy kitchen as they relax on the stools at the bar or lounge in front of the gas fireplace; a nice dimension of ambiance. King sized master offers plenty of room to accommodate house sized furniture. His &amp; her closets lead to a cheater ensuite with double sinks and plenty of cabinetry storage. Work from home! The den is set up for a personal home office with built in cabinets and computer station. Gated over sized walk out patio gives you the sense of having your own backyard! </t>
+  </si>
+  <si>
+    <t>The Ocean</t>
+  </si>
+  <si>
+    <t>A masterpiece in design &amp; quality in prime tower residence in Lower Lakeshore. These suites features 2 bedrooms + Den with view , 2 bathrooms, open floor plan,electric fireplace, in-suite laundry and more. This is only minute away from all the shops, bus, fine restaurants, theatre, waterfront and many more which the city has to offer. Exercise room &amp; Social room at lobby for your healthy lifestyle </t>
+  </si>
+  <si>
+    <t>The Observatory</t>
+  </si>
+  <si>
+    <t>Enjoy coming home to spectacular panoramic views of the Water, City and beyond! Make the "Observatory" your new home and get comfortable in this beautifully renovated 2 bdrm, 2 bath corner units offering only the finest high end materials and finishings. Enjoy cooking in the open custom kitchen offering European S/S appls and fixtures, Limestone floors and many more custom features. Both the bathrooms have also been stunningly updated using only the finest European materials. You will appreciate the sunsets and the views from your oversized sundeck. Relax by the outdoor pool and hot tub or in the beautiful gardens. Conveniently located just steps to top city amenities. </t>
+  </si>
+  <si>
+    <t>The Apartment Store</t>
+  </si>
+  <si>
+    <t>Gorgeous custom designed studio apartments that will be a pleasure to come home to each day. High ceilings, quiet end unit and a patio spacious enough to entertain on during the warmer months. Seascape Landing is a well maintained unassuming building that is ideal for professionals who prefer privacy and less foot traffic than the bigger buildings. </t>
+  </si>
+  <si>
+    <t>McKinnon House</t>
+  </si>
+  <si>
+    <t>Beautifully renovated, extra large one or two bedroom condos at McKinnon House!  Bright and sunny south-facing units with views of Lions Gate Bridge, partial city views and gorgeous sunsets. Renovations include kitchen (cabinets, granite countertops, stainless steel appliances), bathroom (with granite tile flooring), crown mouldings &amp; engineered hardwood throughout. "Other" is den w/ built-ins and granite top desk. Fantastic location in downtown. Enjoy living in this vibrant community - walk to shops, restaurants, parks, public transportation &amp; so much more! One parking spot &amp; one storage locker included. Maintenance fee includes heat and hotwater. </t>
+  </si>
+  <si>
+    <t>The Avenue</t>
+  </si>
+  <si>
+    <t>Beautifully renovated, bright, south facing units in desirable Lower Area. Kitchen is fully updated with white shaker cabinets, quartz countertops, and stainless steel appliances.Open Houses Sun. The dining area flows into a large living room and wrap around balcony. Recent building upgrades include balconies, piping and some patio doors/windows. Grey oak laminate flooring throughout and custom built-in closets in the bedrooms. Healthy contingency fund &amp; attentive Strata Council. Locker and parking included. Rentals allowed &amp; 2 cats welcome. Short walk to bus and shopping on main avenue. </t>
+  </si>
+  <si>
+    <t>The Unique</t>
+  </si>
+  <si>
+    <t>A unique and rare offering - New York style living in this funky building. Lofts are styled most spacious 733 sq. ft home in the heart of the city. With Shops, Restaurants, Recreation &amp; more at your door. Units in this boutique building with live/work status! Run your own business right from home. Open, flexible floor plan with soaring 10 ft ceilings, laminated wood floors &amp; stainless steel appliances-big sliding glass doors opening to a sundrenched private patio. Bonuses galore--gas fireplace, radiant floor heat, cable, internet &amp; management all included in the maintenance fees. Pets allowed too. </t>
+  </si>
+  <si>
+    <t>The Calypso</t>
+  </si>
+  <si>
+    <t>These well-appointed 2B/2B has an excellent layout with a private courtyard entrance and the living area all on the upper level. This floorplan offers a spacious living/dining area, well separated bedrooms, a walk in closet in the master and the nook makes a great office space or eating area. Highlights include laminate floors, a cozy gas fireplace, windows on the east and west side for plenty of natural light and lots of storage space. The location is ideal-walk to the Seabus, restaurants and shops . All this plus 2 side by side prkg stalls and one storage locker in a RAINSCREENED building.</t>
+  </si>
+  <si>
+    <t>Tropical Gardens</t>
+  </si>
+  <si>
+    <t>Charming &amp; quiet inner courtyard 2 bed, 1 bath units. This lovely place is tucked among beautiful tropical gardens &amp; water fountains, an oasis in the middle of the city! Feels just like a townhouse w/a private entrance &amp; large fenced patio. Perfect for children, pets or to enjoy the ocean breeze, peace &amp; serenity! Featuring open concept floor plan &amp; cozy gas fireplace. This unit is in move-in condition with laminated floors, fresh paint &amp; new appliances, incl. washer &amp; dryer. Spacious bathroom with bath tub &amp; separate shower stall for your comfort! All of this is a great fully rain screened bldg &amp; unbeatable location, close to bus, restaurants &amp; shops. 1 Parking &amp; 1 Locker, Don't miss it! </t>
+  </si>
+  <si>
+    <t>The Terrace's Garden</t>
+  </si>
+  <si>
+    <t>All the space you need in a condo that lives like a townhome! These unique condo features a secure courtyard entry to an attractive and spacious SW facing patio. A spectacular reno in this RAINSCREENED building feels like buying a brand new home without the wait, GST or uncertainty. Brand new s/s kitchen appliances and quartz countertops; new designer flooring throughout; a completely reno'd bathroom; front load w&amp;d; all new lighting; fresh designer paint; and custom millwork throughout. Peace of mind knowing of the VERY HEALTHY contingency fund. Huge in-suite storage PLUS external storage locker. NO STAIRS from the secure underground parking to these gorgeous units! </t>
+  </si>
+  <si>
+    <t>The Villas</t>
+  </si>
+  <si>
+    <t>Fabulous Waters Edge. Whisper quiet location in the Villas building. Spacious units 1419 sq ft. Beautiful suites has been lovingly looked after &amp; shows like brand new. High end finishing throughout. 2 outdoor balconies with views to the Capilano River, hardwood flooring, wood carpeting, crown moulding, stainless appliances, Miele, Sub-zero, Hunter Douglas Blinds. 1 parking space &amp; 1 storage locker are included. This elegant property awaiting your viewing appointment. </t>
+  </si>
+  <si>
+    <t>The Water's Edge</t>
+  </si>
+  <si>
+    <t>A rare gem in the city! A building that is rarely available with only one suite per floor! There are panoramic ocean and mountain views from the rooftop deck and terrace. The suites are very spacious, boosting almost 2,000 sqft of living space including: 3 beds, 2.5 baths, living and family rooms, a separate laundry room, and enclosed balcony. The layout is ideal with bedrooms on one side of the suite, and entertaining on the other side. The building is situated on a peaceful and tranquil tree-lined street, just steps from Denman Street, Robson Street, and Stanley Park! With just 14 suites in total, this concrete landmark is loved by its residents. </t>
+  </si>
+  <si>
+    <t>The Arniston</t>
+  </si>
+  <si>
+    <t>Why buy an apartment when you can buy a LIFESTYLE! The Arniston is a crown jewel. These delightful bright suites has been impressively renovated embracing modern styling with classic charm. Gleaming inlaid hardwood oak floors run throughout. A spectacular kitchen that offers high-end stainless appliances, Caesar stone counters and a WINDOW above the sink! Suites have all new windows. Massive living/dining with modern recessed lighting with dimmers to set the mood. City's Best is literally out your front door...You are mere steps to the Sea Wall, Shopping, Restaurants, Library, and so much more. A lifestyle and a home! </t>
+  </si>
+  <si>
+    <t>The Luxury Star</t>
+  </si>
+  <si>
+    <t>Luxurious apartments in the downtown. Georgous views overlooking the lake and High Park, this prime residences features a stunning open floor plan and high end designer touches. Well-appointed, with over 2,100 sq ft of living space including a fabulous Master Suite with walk in closet, private balcony plus additional bedroom. This special condos are an entertainer's delight with a gourmet sized kitchen and balconies off the living room and dining room. Walking distance to shops, restaurants, and recreation, this designer residence won't last long!</t>
+  </si>
+  <si>
+    <t>The City Gardens</t>
+  </si>
+  <si>
+    <t>Most beautiful location. Iconic co-op building Panorama Place is nestled in the end of a cul-de-sac directly beside Stanley Park. Immaculate suites. Generous room sizes. Wall-to-wall windows flood the apartment w/natural light. Walk to the shops &amp; restaurants on main street. Parking, storage &amp; bike storage available. Live-in caretaker. Indoor pool. Common garden for those w/a green thumb. Well maint. &amp; managed building w/ large reserve. Huge rooftop deck w/360 degree view of city's best... water, mountains, parks, city lights, fireworks. Simply amazing. </t>
+  </si>
+  <si>
+    <t>The Pendrell</t>
+  </si>
+  <si>
+    <t>Last building on Pendrell Area. Great opportunity to get into this quality building at an affordable price. Fixer upper needs your TLC to make it yours. Great bones. Everything great about the city is virtually at your door! Imagine sandy beach, golf (pitch &amp; putt) lawn bowling, hiking, biking trails &amp; public tennis courts just an elevator ride away. 2 blocks to shops, grocer &amp; restaurants. 19x 14LR, sep dining (or open den) &amp; king size BR. Well run co-op building w/large reserves. Great lock'go security. Indoor pool. Best view roof deck. 1 cat.</t>
+  </si>
+  <si>
+    <t>The One Room Apartments</t>
+  </si>
+  <si>
+    <t>Large functional 1 bedroom units building. Located overlooking a quiet tree lined street this home features over-height ceilings, gas fireplace, open concept living, huge master, walk-through closet, semi-ensuite, in-suite laundry, large kitchen with pantry, hardwood floors, and an 80 sq ft peaceful balcony. The complex has been extensively updated including full rainscreen, new roof, re-piping, new windows, sliding doors and more over the last 5 years (just in the process of updating lobby and hallways). Steps to parks, dining and shopping. Pets welcome. Units comes with parking and storage. Easy to show and a pleasure. </t>
+  </si>
+  <si>
+    <t>The Friendly Place</t>
+  </si>
+  <si>
+    <t>Fully rainscreened &amp; under warranty, new plumbing, new roof, new windows &amp; refreshed hallways. Very bright units. Great for entertaining w/10'x11' dining area &amp; 14x12 LR. The kitchen has been redesigned to maximize space, lights &amp; function. Upgrades incl new S/S appliances, white Silestone counters &amp; custom cabinets. New engineered hardwood floors throughout, convenient insuite WD &amp; a cozy gas FP too. Sunny balc for BBQ's &amp; sunset martinis. "Walk score 100". Just steps to grocer, shops, restaurants &amp; trans. Beach &amp; park 2 blocks away. 2 pets ok. </t>
+  </si>
+  <si>
+    <t>The Five</t>
+  </si>
+  <si>
+    <t>Top 5 reasons these Condos will not last. 1. LOCATION - downtown. 2. RENOVATIONS - These condos has been FULLY redone. Brand new kitchen includes; new open concept, huge white Quartz countertops, all stainless appl., new w/d, cabinets, pot lights, and back splash. Bathroom includes; new tiles, new cabs &amp; vanity. All new laminate, fresh paint job, &amp; mod. fireplace. 3. LAY-OUT - 1 bed, 1 bath, open kitch/liv, enclosed balcony &amp; large skylight. 4. BUILDING - The Westpark has: a proactive strata, newer roof, new windows, new boiler, siding &amp; balcony upgrades. Pets allowed 5. PRICE – Includes a parking stall and storage locker. </t>
+  </si>
+  <si>
+    <t>Ocean's Bright Light</t>
+  </si>
+  <si>
+    <t>Bright, spacious one or two bedroom units in Prime Location with City and Water Views! Featured include renovated bathroom, double glazed windows, rich dark laminate flooring throughout, newer paint, large balcony, open kitchen, out-door pool &amp; Sauna, storage locker and one rentable parking stall. Maint. fee's include, heat, hot-water, satellite/cable, resident caretaker, management, recreational facilities and property taxes. Just steps to shopping and restaurants </t>
+  </si>
+  <si>
+    <t>Nelson Studios</t>
+  </si>
+  <si>
+    <t>Top studio/Bachelors (not a 1 bedroom) beautifully renovated, 9' ceilings, newer kitchen &amp; bathroom, plus insuite laundry. These units boast a large parking space suitable for SUV's, a storage space, balcony, walk-in closet, hardwood &amp; mexican tile flooring. All this in a well-run building that allows pets &amp; rentals. Excellent location, just steps to the Beach. Perfect for frequent travellers who need a place to hang their hat when in town or for those who wish to help their kids get into the market. Dogs &lt;16" at shoulder. No amount limit. </t>
+  </si>
+  <si>
+    <t>The Palladian</t>
+  </si>
+  <si>
+    <t>The Palladian in the heart of the city, only steps away from  shops, cafes &amp; restaurants. Renovated &amp; updated 2 and 3 bedroom/2 bathroom. Suites over 1070 SF &amp; 2 separate balconies. Spacious plan design features large rooms which accommodate large furniture. Features include in suite laundry, new S/S appliances, Caesarstone kitchen counter tops, paint &amp; flooring. All this is in a rain-screened building &amp; where pets are welcomed. Just move in. </t>
+  </si>
+  <si>
+    <t>The Rain Forest</t>
+  </si>
+  <si>
+    <t>1 bdrm suites with windows galore! Sunny, bright &amp; cozy. Walk score 95 - a walker's paradise close to Downtown. A transit score of 96 &amp; good bike lanes mean your car may rarely leave the included parking stall. One of the few  buildings with a gas fireplace. Good flow through separate dining &amp; living rooms. Includes extra large bathtub. Well managed building with a pro-active strata will soon be re-piped. Seller already paid. 3 exterior walls rainscreened. Several balcony upgrades. Amenities: guest parking, onsite caretaker, sauna/fitness room. Pets &amp; rentals okay. Locker included. See it &amp; fall in love! </t>
+  </si>
+  <si>
+    <t>The Beam</t>
+  </si>
+  <si>
+    <t>Construction offers overheight ceilings, no bearing walls appealing to creative lifestyles. Rough beams warehouse style, can be stripped, boxed. 9 ft ceilings add to feeling of space. Spacious one bedroom units with office nook, extra large cook's kitchen and gracious living/dining areas for entertaining. Recent paint, blinds &amp; laminate flooring. Updated bath. Good storage, underground parking. Large balcony overlooking peaceful quiet garden &amp; only one common wall! Laundry can be installed with strata permission. </t>
+  </si>
+  <si>
+    <t>The Westport</t>
+  </si>
+  <si>
+    <t>Just steps away from all that the West End has to offer, this bright suites at the WESTPORT features a spacious living room and enclosed balcony - perfect for home office or reading room (included in sqft). Recently painted, these suites are carpeted throughout with newer floor tile in both kitchen and bathroom. The kitchens are clean, original condition with ample storage/counter space &amp; newer appliances. Other UPGRADES include newer tile around bathtub. The bedrooms will easily accommodate a queen sized bed and furniture. BUILDING UPGRADES include rainscreening, newer windows &amp; new balconies. AMENITIES include shared laundry, sauna/fitness room + live in caretaker. Suite incl parking/locker. </t>
+  </si>
+  <si>
+    <t>The Barclay</t>
+  </si>
+  <si>
+    <t>The Barclay is in the heart of the West End in city's most established, diverse, &amp; vibrant neighbourhood. Located just blocks away from shopping. These large 1 bedroom units feature huge outdoor sundrenched patio perfect for entertaining and enjoying the West End. Features include: granite countertops, laminate floors, &amp; tiled kitchens, entrances, &amp; hallways. Perfect for any first time buyer or investor. Units include parking and storage locker. These won't last long come soon. </t>
+  </si>
+  <si>
+    <t>Bayshore Gardens I</t>
+  </si>
+  <si>
+    <t>Exclusive "Bayshore Gardens" tower. Quite, Elegant and High Potential Value. This bright 2 bedroom and den condos brings a view with coal harbour Marina, High Park and North Shore Mountains. Also trees surrounding to keep privacy perfectly protected. Excellent layout with open kitchen plan featuring granite countertops, high-end appliances, gas fireplace, air conditioning, oversize balcony with lovely view. 24 hour concierge service and health club. 1 parking and 1 locker included. Don't MISS! </t>
+  </si>
+  <si>
+    <t>Bayshore Gardens II</t>
+  </si>
+  <si>
+    <t>Rare opportunity to own your home in prestigious Bayshore Garden. Excellent waterfront location. Great view of marina, park &amp; mountain from unit. These luxurious 1, 2 and 3 bedroom plus den with 2 bathroom unit features gourment kitchen with granite countertops, large size of kitchen island. Bosch &amp; Sub-zero appliance and BBQ on the large covered balcony, gas range and fireplace. Large in-suite storage room, air conditioning, 24 hours concierge, Well-Maintanced building. Enjoy the comforts of resort style living in the heart of harbour. Walking distance to parks, beaches, restaurants and world famous seawall. Please to show. </t>
+  </si>
+  <si>
+    <t>The Coal</t>
+  </si>
+  <si>
+    <t>A location like no other... 3 level townhouse just steps from seawall and park. Convenience is an understatement! Beautiful units with an extensive renovation including: Riobel ishower with full media, heated floors, Toto Neorest, new custom kitchen and bath cabinetry, custom wood surround fireplace, full granite backsplash, California closets, new front load washer dryer, plush carpets, Wolf cooktop, wine fridge, all media wired, nest thermostat and smoke detection system to control the home wirelessly and remotely optionally. Units like this rarely come available. </t>
+  </si>
+  <si>
+    <t>The City Water</t>
+  </si>
+  <si>
+    <t>Stunning City, Water &amp; Mountain Views from all units in this Executive residence's building! One of a kind floor plan! Highlights include 5 balconies per floor in total (including 2 that are extra large), den/flex space, 24 hour concierge service, sizable walk-in closet, 2 side-by-side parking stalls and a storage locker. This space is sure to impress!  Walking distance to  Lift Bar &amp; Grill. Contact the agent for a private viewing. </t>
   </si>
 </sst>
 </file>
@@ -329,10 +755,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A87" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A89" activeCellId="0" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -469,6 +895,574 @@
         <v>31</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="132.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="168.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="156.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="192.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="144.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="132.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="192.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="192.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="192.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="168.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="192.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="156.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="144.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="132.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="168.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="132.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="132.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="252.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="300" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="311.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="288.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="144.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="288.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="264.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="252.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="252.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="300" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="300" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="276.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="276.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="228.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="240.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="228.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="264.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="240.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="288.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="228.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="264.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="228.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="311.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="276.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="240.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>